<commit_message>
Complete Menu UI, Car Selection
</commit_message>
<xml_diff>
--- a/Tiến độ project thực tập.xlsx
+++ b/Tiến độ project thực tập.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\Unity tamj\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TDQ DATA\GIT\COLOR-RACING-PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683A58D2-BB75-400B-B739-50508127E09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29649D37-846D-4EF8-903E-2BB59E4936FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11835" xr2:uid="{3574CA86-C1E3-4B87-924A-3D593C3DD8F2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t>Build Begiiner Basic</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Cutscenes</t>
   </si>
   <si>
-    <t>Minimap &amp; New track</t>
-  </si>
-  <si>
     <t>Car Selection &amp; Customize</t>
   </si>
   <si>
@@ -103,6 +100,12 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>New track</t>
+  </si>
+  <si>
+    <t>Minimap</t>
   </si>
 </sst>
 </file>
@@ -487,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E408A510-748A-4A7C-A53E-FBE13F08E3E4}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,10 +504,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
@@ -512,7 +515,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
@@ -520,7 +523,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
@@ -528,7 +531,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
@@ -536,7 +539,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
@@ -544,7 +547,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
@@ -552,7 +555,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
@@ -560,7 +563,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
@@ -568,7 +571,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
@@ -576,7 +579,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
@@ -584,7 +587,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
@@ -592,62 +595,74 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="15" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="16" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" s="1"/>
     </row>
     <row r="17" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" s="1"/>
     </row>
     <row r="18" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" s="1"/>
     </row>
     <row r="19" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19" s="1"/>
     </row>
     <row r="20" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1"/>
     </row>
     <row r="21" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A21" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1"/>
+    </row>
+    <row r="22" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add bgm, saving cash, saving car bought
</commit_message>
<xml_diff>
--- a/Tiến độ project thực tập.xlsx
+++ b/Tiến độ project thực tập.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TDQ DATA\GIT\COLOR-RACING-PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDDEB8A8-18A8-4C75-889D-E38533EAE7C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFB151B0-F93F-4A60-B094-35DDAFF0BF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13152" xr2:uid="{3574CA86-C1E3-4B87-924A-3D593C3DD8F2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3574CA86-C1E3-4B87-924A-3D593C3DD8F2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>Build Begiiner Basic</t>
   </si>
@@ -106,12 +106,6 @@
   </si>
   <si>
     <t>Minimap</t>
-  </si>
-  <si>
-    <t>IN PROGRESS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PHẦN CHỌN MÀU VÀ POSITION VẪN CÒN LỖI VÀ EM ĐANG HOÀN THIỆN Ạ </t>
   </si>
 </sst>
 </file>
@@ -175,7 +169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -183,6 +177,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -499,19 +496,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E408A510-748A-4A7C-A53E-FBE13F08E3E4}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8:Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.5703125" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="45.5546875" customWidth="1"/>
+    <col min="2" max="2" width="27.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -519,7 +516,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -527,7 +524,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -535,7 +532,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -543,7 +540,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -551,7 +548,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -559,7 +556,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -567,23 +564,45 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+    </row>
+    <row r="9" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+    </row>
+    <row r="10" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -591,7 +610,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -599,7 +618,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -607,7 +626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -615,7 +634,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -623,7 +642,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -631,7 +650,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:17" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A16" s="1" t="s">
         <v>12</v>
       </c>
@@ -639,48 +658,52 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B20" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A21" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="1:6" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:6" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A22" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>25</v>
-      </c>
+    <row r="23" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
@@ -688,8 +711,9 @@
       <c r="F23" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A23:F23"/>
+    <mergeCell ref="G8:Q9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>